<commit_message>
chart complete but not 100% yet
</commit_message>
<xml_diff>
--- a/num.xlsx
+++ b/num.xlsx
@@ -68,6 +68,823 @@
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$C$2:$C$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$C$2:$C$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$C$2:$C$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>'Sheet1'!$C$2:$C$34</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$C$2:$C$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$C$2:$C$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="5" name="Chart 5"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="6" name="Chart 6"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -332,7 +1149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1690,12 +2507,12 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="1" t="inlineStr">
         <is>
           <t>Median:</t>
         </is>
       </c>
-      <c r="B36" t="n">
+      <c r="B36" s="1" t="n">
         <v>40</v>
       </c>
     </row>
@@ -1710,36 +2527,37 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="1" t="inlineStr">
         <is>
           <t>Min:</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="B38" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="1" t="inlineStr">
         <is>
           <t>Standard Deviation:</t>
         </is>
       </c>
-      <c r="B39" t="n">
+      <c r="B39" s="1" t="n">
         <v>20.77276042700093</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="1" t="inlineStr">
         <is>
           <t>Variance:</t>
         </is>
       </c>
-      <c r="B40" t="n">
+      <c r="B40" s="1" t="n">
         <v>431.5075757575758</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add user input for controlling the chart
</commit_message>
<xml_diff>
--- a/num.xlsx
+++ b/num.xlsx
@@ -750,6 +750,351 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$C$2:$C$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$B$2:$B$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$C$2:$C$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$B$2:$B$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$B$2:$B$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -879,6 +1224,72 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="7" name="Chart 7"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="8" name="Chart 8"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="9" name="Chart 9"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -2503,7 +2914,7 @@
         </is>
       </c>
       <c r="B35" s="1" t="n">
-        <v>43.15151515151515</v>
+        <v>32172918.09090909</v>
       </c>
     </row>
     <row r="36">
@@ -2513,7 +2924,7 @@
         </is>
       </c>
       <c r="B36" s="1" t="n">
-        <v>40</v>
+        <v>32180213</v>
       </c>
     </row>
     <row r="37">
@@ -2523,7 +2934,7 @@
         </is>
       </c>
       <c r="B37" s="1" t="n">
-        <v>84</v>
+        <v>32184559</v>
       </c>
     </row>
     <row r="38">
@@ -2533,7 +2944,7 @@
         </is>
       </c>
       <c r="B38" s="1" t="n">
-        <v>2</v>
+        <v>32132203</v>
       </c>
     </row>
     <row r="39">
@@ -2543,7 +2954,7 @@
         </is>
       </c>
       <c r="B39" s="1" t="n">
-        <v>20.77276042700093</v>
+        <v>11997.82486631336</v>
       </c>
     </row>
     <row r="40">
@@ -2553,7 +2964,7 @@
         </is>
       </c>
       <c r="B40" s="1" t="n">
-        <v>431.5075757575758</v>
+        <v>143947801.5227273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Todo list on project file
</commit_message>
<xml_diff>
--- a/num.xlsx
+++ b/num.xlsx
@@ -71,6 +71,236 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$C$2:$C$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$B$2:$B$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -1295,6 +1525,50 @@
     </graphicFrame>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="10" name="Chart 10"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="11" name="Chart 11"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -2914,7 +3188,7 @@
         </is>
       </c>
       <c r="B35" s="1" t="n">
-        <v>32172918.09090909</v>
+        <v>43.15151515151515</v>
       </c>
     </row>
     <row r="36">
@@ -2924,7 +3198,7 @@
         </is>
       </c>
       <c r="B36" s="1" t="n">
-        <v>32180213</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37">
@@ -2934,7 +3208,7 @@
         </is>
       </c>
       <c r="B37" s="1" t="n">
-        <v>32184559</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38">
@@ -2944,7 +3218,7 @@
         </is>
       </c>
       <c r="B38" s="1" t="n">
-        <v>32132203</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -2954,7 +3228,7 @@
         </is>
       </c>
       <c r="B39" s="1" t="n">
-        <v>11997.82486631336</v>
+        <v>20.77276042700093</v>
       </c>
     </row>
     <row r="40">
@@ -2964,7 +3238,7 @@
         </is>
       </c>
       <c r="B40" s="1" t="n">
-        <v>143947801.5227273</v>
+        <v>431.5075757575758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a new file
</commit_message>
<xml_diff>
--- a/num.xlsx
+++ b/num.xlsx
@@ -301,6 +301,351 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$C$2:$C$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$C$2:$C$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Number Theory 2019 Middle Term</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>2019 중간고사 성적</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet1'!$C$2:$C$34</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$34</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 이름</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>학생 성적</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -1564,6 +1909,72 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="12" name="Chart 12"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="13" name="Chart 13"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="14" name="Chart 14"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId14"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>

</xml_diff>

<commit_message>
Add user input for chart location in excel
</commit_message>
<xml_diff>
--- a/num.xlsx
+++ b/num.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7710" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7716" windowWidth="20496" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -77,6 +77,7 @@
       <tx>
         <rich>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
@@ -87,9 +88,13 @@
           </a:p>
         </rich>
       </tx>
+      <overlay val="0"/>
     </title>
     <plotArea>
+      <layout/>
       <scatterChart>
+        <scatterStyle val="lineMarker"/>
+        <varyColors val="0"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
@@ -110,16 +115,230 @@
             </spPr>
           </marker>
           <xVal>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$34</f>
-            </numRef>
+            <strRef>
+              <f>Sheet1!$C$2:$C$34</f>
+              <strCache>
+                <ptCount val="33"/>
+                <pt idx="0">
+                  <v>고영민</v>
+                </pt>
+                <pt idx="1">
+                  <v>구동근</v>
+                </pt>
+                <pt idx="2">
+                  <v>김건휘</v>
+                </pt>
+                <pt idx="3">
+                  <v>김명서</v>
+                </pt>
+                <pt idx="4">
+                  <v>김승국</v>
+                </pt>
+                <pt idx="5">
+                  <v>김영웅</v>
+                </pt>
+                <pt idx="6">
+                  <v>김영호</v>
+                </pt>
+                <pt idx="7">
+                  <v>김재원</v>
+                </pt>
+                <pt idx="8">
+                  <v>김정선</v>
+                </pt>
+                <pt idx="9">
+                  <v>김하경</v>
+                </pt>
+                <pt idx="10">
+                  <v>김현진</v>
+                </pt>
+                <pt idx="11">
+                  <v>김혜련</v>
+                </pt>
+                <pt idx="12">
+                  <v>노희성</v>
+                </pt>
+                <pt idx="13">
+                  <v>류가은</v>
+                </pt>
+                <pt idx="14">
+                  <v>박건희</v>
+                </pt>
+                <pt idx="15">
+                  <v>박세진</v>
+                </pt>
+                <pt idx="16">
+                  <v>박지은</v>
+                </pt>
+                <pt idx="17">
+                  <v>박찬우</v>
+                </pt>
+                <pt idx="18">
+                  <v>배기란</v>
+                </pt>
+                <pt idx="19">
+                  <v>설예지</v>
+                </pt>
+                <pt idx="20">
+                  <v>오영훈</v>
+                </pt>
+                <pt idx="21">
+                  <v>이승재</v>
+                </pt>
+                <pt idx="22">
+                  <v>이주미</v>
+                </pt>
+                <pt idx="23">
+                  <v>임동민</v>
+                </pt>
+                <pt idx="24">
+                  <v>장시은</v>
+                </pt>
+                <pt idx="25">
+                  <v>장욱진</v>
+                </pt>
+                <pt idx="26">
+                  <v>정문성</v>
+                </pt>
+                <pt idx="27">
+                  <v>조우창</v>
+                </pt>
+                <pt idx="28">
+                  <v>조원희</v>
+                </pt>
+                <pt idx="29">
+                  <v>진정택</v>
+                </pt>
+                <pt idx="30">
+                  <v>최미진</v>
+                </pt>
+                <pt idx="31">
+                  <v>최승혁</v>
+                </pt>
+                <pt idx="32">
+                  <v>허성빈</v>
+                </pt>
+              </strCache>
+            </strRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>'Sheet1'!$A$2:$A$34</f>
+              <f>Sheet1!$A$2:$A$34</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="33"/>
+                <pt idx="0">
+                  <v>72</v>
+                </pt>
+                <pt idx="1">
+                  <v>62</v>
+                </pt>
+                <pt idx="2">
+                  <v>40</v>
+                </pt>
+                <pt idx="3">
+                  <v>24</v>
+                </pt>
+                <pt idx="4">
+                  <v>26</v>
+                </pt>
+                <pt idx="5">
+                  <v>30</v>
+                </pt>
+                <pt idx="6">
+                  <v>30</v>
+                </pt>
+                <pt idx="7">
+                  <v>22</v>
+                </pt>
+                <pt idx="8">
+                  <v>56</v>
+                </pt>
+                <pt idx="9">
+                  <v>42</v>
+                </pt>
+                <pt idx="10">
+                  <v>50</v>
+                </pt>
+                <pt idx="11">
+                  <v>14</v>
+                </pt>
+                <pt idx="12">
+                  <v>48</v>
+                </pt>
+                <pt idx="13">
+                  <v>60</v>
+                </pt>
+                <pt idx="14">
+                  <v>40</v>
+                </pt>
+                <pt idx="15">
+                  <v>78</v>
+                </pt>
+                <pt idx="16">
+                  <v>48</v>
+                </pt>
+                <pt idx="17">
+                  <v>38</v>
+                </pt>
+                <pt idx="18">
+                  <v>2</v>
+                </pt>
+                <pt idx="19">
+                  <v>40</v>
+                </pt>
+                <pt idx="20">
+                  <v>84</v>
+                </pt>
+                <pt idx="21">
+                  <v>64</v>
+                </pt>
+                <pt idx="22">
+                  <v>32</v>
+                </pt>
+                <pt idx="23">
+                  <v>34</v>
+                </pt>
+                <pt idx="24">
+                  <v>78</v>
+                </pt>
+                <pt idx="25">
+                  <v>34</v>
+                </pt>
+                <pt idx="26">
+                  <v>62</v>
+                </pt>
+                <pt idx="27">
+                  <v>48</v>
+                </pt>
+                <pt idx="28">
+                  <v>14</v>
+                </pt>
+                <pt idx="29">
+                  <v>10</v>
+                </pt>
+                <pt idx="30">
+                  <v>24</v>
+                </pt>
+                <pt idx="31">
+                  <v>58</v>
+                </pt>
+                <pt idx="32">
+                  <v>60</v>
+                </pt>
+              </numCache>
             </numRef>
           </yVal>
+          <smooth val="0"/>
         </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
         <axId val="10"/>
         <axId val="20"/>
       </scatterChart>
@@ -128,12 +347,14 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <axPos val="l"/>
+        <delete val="0"/>
+        <axPos val="b"/>
         <majorGridlines/>
         <title>
           <tx>
             <rich>
               <a:bodyPr/>
+              <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr/>
@@ -144,22 +365,28 @@
               </a:p>
             </rich>
           </tx>
+          <overlay val="0"/>
         </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
         <crossAx val="20"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="midCat"/>
       </valAx>
       <valAx>
         <axId val="20"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
+        <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
         <title>
           <tx>
             <rich>
               <a:bodyPr/>
+              <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr/>
@@ -170,589 +397,20 @@
               </a:p>
             </rich>
           </tx>
+          <overlay val="0"/>
         </title>
+        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
         <crossAx val="10"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="midCat"/>
       </valAx>
     </plotArea>
     <legend>
       <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet1'!$B$2:$B$34</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet1'!$A$2:$A$34</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 이름</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$34</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet1'!$A$2:$A$34</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 이름</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$34</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet1'!$A$2:$A$34</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 이름</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$34</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet1'!$A$2:$A$34</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 이름</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$34</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet1'!$A$2:$A$34</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 이름</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
+      <overlay val="0"/>
     </legend>
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
@@ -990,693 +648,13 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>'Sheet1'!$C$2:$C$34</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$34</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet1'!$A$2:$A$34</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 이름</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$34</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet1'!$A$2:$A$34</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 이름</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$34</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet1'!$B$2:$B$34</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 이름</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$34</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet1'!$B$2:$B$34</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 이름</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet1'!$A$2:$A$34</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet1'!$B$2:$B$34</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 이름</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>4</col>
+      <col>139</col>
       <colOff>0</colOff>
-      <row>35</row>
+      <row>39</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -1696,9 +674,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>4</col>
+      <col>139</col>
       <colOff>0</colOff>
-      <row>35</row>
+      <row>34</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -1718,9 +696,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>4</col>
+      <col>9</col>
       <colOff>0</colOff>
-      <row>35</row>
+      <row>39</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -1733,248 +711,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="4" name="Chart 4"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="5" name="Chart 5"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="6" name="Chart 6"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId6"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="7" name="Chart 7"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId7"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="8" name="Chart 8"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId8"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="9" name="Chart 9"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId9"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="10" name="Chart 10"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId10"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="11" name="Chart 11"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId11"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="12" name="Chart 12"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId12"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="13" name="Chart 13"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId13"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="14" name="Chart 14"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId14"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -2252,11 +988,11 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="17.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">

</xml_diff>

<commit_message>
able to save graphs and add into the excel file
</commit_message>
<xml_diff>
--- a/num.xlsx
+++ b/num.xlsx
@@ -425,6 +425,7 @@
       <tx>
         <rich>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
@@ -435,9 +436,13 @@
           </a:p>
         </rich>
       </tx>
+      <overlay val="0"/>
     </title>
     <plotArea>
+      <layout/>
       <scatterChart>
+        <scatterStyle val="lineMarker"/>
+        <varyColors val="0"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
@@ -458,16 +463,230 @@
             </spPr>
           </marker>
           <xVal>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$34</f>
-            </numRef>
+            <strRef>
+              <f>Sheet1!$C$2:$C$34</f>
+              <strCache>
+                <ptCount val="33"/>
+                <pt idx="0">
+                  <v>고영민</v>
+                </pt>
+                <pt idx="1">
+                  <v>구동근</v>
+                </pt>
+                <pt idx="2">
+                  <v>김건휘</v>
+                </pt>
+                <pt idx="3">
+                  <v>김명서</v>
+                </pt>
+                <pt idx="4">
+                  <v>김승국</v>
+                </pt>
+                <pt idx="5">
+                  <v>김영웅</v>
+                </pt>
+                <pt idx="6">
+                  <v>김영호</v>
+                </pt>
+                <pt idx="7">
+                  <v>김재원</v>
+                </pt>
+                <pt idx="8">
+                  <v>김정선</v>
+                </pt>
+                <pt idx="9">
+                  <v>김하경</v>
+                </pt>
+                <pt idx="10">
+                  <v>김현진</v>
+                </pt>
+                <pt idx="11">
+                  <v>김혜련</v>
+                </pt>
+                <pt idx="12">
+                  <v>노희성</v>
+                </pt>
+                <pt idx="13">
+                  <v>류가은</v>
+                </pt>
+                <pt idx="14">
+                  <v>박건희</v>
+                </pt>
+                <pt idx="15">
+                  <v>박세진</v>
+                </pt>
+                <pt idx="16">
+                  <v>박지은</v>
+                </pt>
+                <pt idx="17">
+                  <v>박찬우</v>
+                </pt>
+                <pt idx="18">
+                  <v>배기란</v>
+                </pt>
+                <pt idx="19">
+                  <v>설예지</v>
+                </pt>
+                <pt idx="20">
+                  <v>오영훈</v>
+                </pt>
+                <pt idx="21">
+                  <v>이승재</v>
+                </pt>
+                <pt idx="22">
+                  <v>이주미</v>
+                </pt>
+                <pt idx="23">
+                  <v>임동민</v>
+                </pt>
+                <pt idx="24">
+                  <v>장시은</v>
+                </pt>
+                <pt idx="25">
+                  <v>장욱진</v>
+                </pt>
+                <pt idx="26">
+                  <v>정문성</v>
+                </pt>
+                <pt idx="27">
+                  <v>조우창</v>
+                </pt>
+                <pt idx="28">
+                  <v>조원희</v>
+                </pt>
+                <pt idx="29">
+                  <v>진정택</v>
+                </pt>
+                <pt idx="30">
+                  <v>최미진</v>
+                </pt>
+                <pt idx="31">
+                  <v>최승혁</v>
+                </pt>
+                <pt idx="32">
+                  <v>허성빈</v>
+                </pt>
+              </strCache>
+            </strRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>'Sheet1'!$A$2:$A$34</f>
+              <f>Sheet1!$A$2:$A$34</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="33"/>
+                <pt idx="0">
+                  <v>72</v>
+                </pt>
+                <pt idx="1">
+                  <v>62</v>
+                </pt>
+                <pt idx="2">
+                  <v>40</v>
+                </pt>
+                <pt idx="3">
+                  <v>24</v>
+                </pt>
+                <pt idx="4">
+                  <v>26</v>
+                </pt>
+                <pt idx="5">
+                  <v>30</v>
+                </pt>
+                <pt idx="6">
+                  <v>30</v>
+                </pt>
+                <pt idx="7">
+                  <v>22</v>
+                </pt>
+                <pt idx="8">
+                  <v>56</v>
+                </pt>
+                <pt idx="9">
+                  <v>42</v>
+                </pt>
+                <pt idx="10">
+                  <v>50</v>
+                </pt>
+                <pt idx="11">
+                  <v>14</v>
+                </pt>
+                <pt idx="12">
+                  <v>48</v>
+                </pt>
+                <pt idx="13">
+                  <v>60</v>
+                </pt>
+                <pt idx="14">
+                  <v>40</v>
+                </pt>
+                <pt idx="15">
+                  <v>78</v>
+                </pt>
+                <pt idx="16">
+                  <v>48</v>
+                </pt>
+                <pt idx="17">
+                  <v>38</v>
+                </pt>
+                <pt idx="18">
+                  <v>2</v>
+                </pt>
+                <pt idx="19">
+                  <v>40</v>
+                </pt>
+                <pt idx="20">
+                  <v>84</v>
+                </pt>
+                <pt idx="21">
+                  <v>64</v>
+                </pt>
+                <pt idx="22">
+                  <v>32</v>
+                </pt>
+                <pt idx="23">
+                  <v>34</v>
+                </pt>
+                <pt idx="24">
+                  <v>78</v>
+                </pt>
+                <pt idx="25">
+                  <v>34</v>
+                </pt>
+                <pt idx="26">
+                  <v>62</v>
+                </pt>
+                <pt idx="27">
+                  <v>48</v>
+                </pt>
+                <pt idx="28">
+                  <v>14</v>
+                </pt>
+                <pt idx="29">
+                  <v>10</v>
+                </pt>
+                <pt idx="30">
+                  <v>24</v>
+                </pt>
+                <pt idx="31">
+                  <v>58</v>
+                </pt>
+                <pt idx="32">
+                  <v>60</v>
+                </pt>
+              </numCache>
             </numRef>
           </yVal>
+          <smooth val="0"/>
         </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
         <axId val="10"/>
         <axId val="20"/>
       </scatterChart>
@@ -476,12 +695,14 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <axPos val="l"/>
+        <delete val="0"/>
+        <axPos val="b"/>
         <majorGridlines/>
         <title>
           <tx>
             <rich>
               <a:bodyPr/>
+              <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr/>
@@ -492,22 +713,28 @@
               </a:p>
             </rich>
           </tx>
+          <overlay val="0"/>
         </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
         <crossAx val="20"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="midCat"/>
       </valAx>
       <valAx>
         <axId val="20"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
+        <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
         <title>
           <tx>
             <rich>
               <a:bodyPr/>
+              <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr/>
@@ -518,129 +745,20 @@
               </a:p>
             </rich>
           </tx>
+          <overlay val="0"/>
         </title>
+        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
         <crossAx val="10"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="midCat"/>
       </valAx>
     </plotArea>
     <legend>
       <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Number Theory 2019 Middle Term</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>2019 중간고사 성적</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$34</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet1'!$A$2:$A$34</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 이름</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>학생 성적</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
+      <overlay val="0"/>
     </legend>
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
@@ -698,22 +816,50 @@
     <from>
       <col>9</col>
       <colOff>0</colOff>
-      <row>39</row>
+      <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="3" name="Chart 3"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="3" name="Image 3"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>16</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="4" name="Image 4"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
     <clientData/>
   </oneCellAnchor>
 </wsDr>
@@ -988,7 +1134,7 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
rewrite some hangul snentences
</commit_message>
<xml_diff>
--- a/num.xlsx
+++ b/num.xlsx
@@ -833,6 +833,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -852,6 +855,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="5" name="Image 5"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>49</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="6" name="Image 6"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>

</xml_diff>

<commit_message>
Need to look at Project.py
</commit_message>
<xml_diff>
--- a/num.xlsx
+++ b/num.xlsx
@@ -887,6 +887,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="6" name="Image 6"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>

</xml_diff>